<commit_message>
small changes in HEV
</commit_message>
<xml_diff>
--- a/ERROR_BY_YEAR.xlsx
+++ b/ERROR_BY_YEAR.xlsx
@@ -7,23 +7,20 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="2013" sheetId="1" r:id="rId1"/>
-    <sheet name="2014" sheetId="2" r:id="rId2"/>
-    <sheet name="2015" sheetId="3" r:id="rId3"/>
-    <sheet name="2016" sheetId="4" r:id="rId4"/>
-    <sheet name="2017" sheetId="5" r:id="rId5"/>
-    <sheet name="2018" sheetId="6" r:id="rId6"/>
-    <sheet name="2019" sheetId="7" r:id="rId7"/>
-    <sheet name="2020" sheetId="8" r:id="rId8"/>
+    <sheet name="2016" sheetId="1" r:id="rId1"/>
+    <sheet name="2017" sheetId="2" r:id="rId2"/>
+    <sheet name="2018" sheetId="3" r:id="rId3"/>
+    <sheet name="2019" sheetId="4" r:id="rId4"/>
+    <sheet name="2020" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
-  <si>
-    <t>sales country</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+  <si>
+    <t>SALES_COUNTRY</t>
   </si>
   <si>
     <t>oem group</t>
@@ -35,30 +32,12 @@
     <t>make model</t>
   </si>
   <si>
-    <t>sum_computed_2013</t>
+    <t>sum_computed_2016</t>
   </si>
   <si>
     <t>diff</t>
   </si>
   <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>sum_computed_2014</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>sum_computed_2015</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>sum_computed_2016</t>
-  </si>
-  <si>
     <t>2016</t>
   </si>
   <si>
@@ -68,33 +47,12 @@
     <t>2017</t>
   </si>
   <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>R-N-M Alliance</t>
-  </si>
-  <si>
-    <t>Nissan</t>
-  </si>
-  <si>
-    <t>Nissan e-NV200 EV</t>
-  </si>
-  <si>
     <t>sum_computed_2018</t>
   </si>
   <si>
     <t>2018</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Unspec.</t>
-  </si>
-  <si>
-    <t>Unspec. LCVs</t>
-  </si>
-  <si>
     <t>sum_computed_2019</t>
   </si>
   <si>
@@ -105,24 +63,6 @@
   </si>
   <si>
     <t>2020</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Luxembourg</t>
-  </si>
-  <si>
-    <t>Daimler AG</t>
-  </si>
-  <si>
-    <t>Mercedes-Benz</t>
-  </si>
-  <si>
-    <t>Mercedes eSprinter Van EV</t>
-  </si>
-  <si>
-    <t>Mercedes GLA250e PHEV</t>
   </si>
 </sst>
 </file>
@@ -644,140 +584,6 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>4958</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>422</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2">
-        <v>40094.2890651</v>
-      </c>
-      <c r="G2">
-        <v>5.099995178170502E-06</v>
-      </c>
-      <c r="H2">
-        <v>40094.28906</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -803,106 +609,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>2596</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>4275</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>